<commit_message>
Changes to google scholars
</commit_message>
<xml_diff>
--- a/Slides/Tex/lecture_includes/google_scholar_did.xlsx
+++ b/Slides/Tex/lecture_includes/google_scholar_did.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Causal-Inference-2/Slides/Tex/lecture_includes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scunning/Causal-Inference-2/Slides/Tex/lecture_includes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAC7E83-99E9-F44B-B6D9-1EB132543DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A2D525-9555-CB4D-B069-9D7237838DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36140" yWindow="500" windowWidth="34420" windowHeight="21100" xr2:uid="{4E948A00-989C-8C4A-9363-AFB9B32B4834}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20320" xr2:uid="{4E948A00-989C-8C4A-9363-AFB9B32B4834}"/>
   </bookViews>
   <sheets>
     <sheet name="PT DID" sheetId="1" r:id="rId1"/>
@@ -101,15 +101,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,13 +129,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1575,7 +1634,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1590,19 +1649,19 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1622,19 +1681,19 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
         <v>0</v>
       </c>
       <c r="G2">
         <v>286</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1648,19 +1707,19 @@
       <c r="C3">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3">
         <v>357</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1674,19 +1733,19 @@
       <c r="C4">
         <v>18</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
         <v>0</v>
       </c>
       <c r="G4">
         <v>405</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1700,19 +1759,19 @@
       <c r="C5">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
         <v>0</v>
       </c>
       <c r="G5">
         <v>476</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1726,19 +1785,19 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6">
         <v>487</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1752,19 +1811,19 @@
       <c r="C7">
         <v>26</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
         <v>0</v>
       </c>
       <c r="G7">
         <v>538</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1778,19 +1837,19 @@
       <c r="C8">
         <v>49</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8">
         <v>627</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1804,19 +1863,19 @@
       <c r="C9">
         <v>47</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9">
         <v>663</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1830,23 +1889,23 @@
       <c r="C10">
         <v>88</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>2</v>
       </c>
       <c r="G10">
         <v>696</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1999</v>
       </c>
@@ -1856,45 +1915,45 @@
       <c r="C11">
         <v>103</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11">
         <v>802</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>2000</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>345</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>147</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
         <v>3</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>971</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1908,19 +1967,19 @@
       <c r="C13">
         <v>189</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
         <v>5</v>
       </c>
       <c r="G13">
         <v>1100</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1934,19 +1993,19 @@
       <c r="C14">
         <v>246</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
         <v>4</v>
       </c>
       <c r="G14">
         <v>1120</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1960,19 +2019,19 @@
       <c r="C15">
         <v>379</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="9">
         <v>2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>8</v>
       </c>
       <c r="G15">
         <v>1460</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1986,19 +2045,19 @@
       <c r="C16">
         <v>535</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
         <v>5</v>
       </c>
       <c r="G16">
         <v>1340</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>9</v>
       </c>
     </row>
@@ -2012,19 +2071,19 @@
       <c r="C17">
         <v>537</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>3</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
         <v>17</v>
       </c>
       <c r="G17">
         <v>1490</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>9</v>
       </c>
     </row>
@@ -2038,19 +2097,19 @@
       <c r="C18">
         <v>733</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>4</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>22</v>
       </c>
       <c r="G18">
         <v>1620</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>20</v>
       </c>
     </row>
@@ -2064,19 +2123,19 @@
       <c r="C19">
         <v>933</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>13</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="11">
         <v>2</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>22</v>
       </c>
       <c r="G19">
         <v>1840</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>21</v>
       </c>
     </row>
@@ -2090,19 +2149,19 @@
       <c r="C20">
         <v>1180</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>15</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="11">
         <v>2</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>33</v>
       </c>
       <c r="G20">
         <v>1930</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>27</v>
       </c>
     </row>
@@ -2116,19 +2175,19 @@
       <c r="C21">
         <v>1370</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>28</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="11">
         <v>4</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>46</v>
       </c>
       <c r="G21">
         <v>2140</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>27</v>
       </c>
     </row>
@@ -2142,19 +2201,19 @@
       <c r="C22">
         <v>1670</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>41</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="11">
         <v>2</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>52</v>
       </c>
       <c r="G22">
         <v>2330</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>37</v>
       </c>
     </row>
@@ -2168,19 +2227,19 @@
       <c r="C23">
         <v>2100</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>48</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="11">
         <v>8</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>71</v>
       </c>
       <c r="G23">
         <v>2640</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>68</v>
       </c>
     </row>
@@ -2194,19 +2253,19 @@
       <c r="C24">
         <v>2620</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>61</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="11">
         <v>11</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>112</v>
       </c>
       <c r="G24">
         <v>3000</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>67</v>
       </c>
     </row>
@@ -2220,19 +2279,19 @@
       <c r="C25">
         <v>3020</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>136</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="11">
         <v>19</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>132</v>
       </c>
       <c r="G25">
         <v>3190</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>114</v>
       </c>
     </row>
@@ -2246,19 +2305,19 @@
       <c r="C26">
         <v>3790</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>209</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="11">
         <v>34</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>184</v>
       </c>
       <c r="G26">
         <v>3540</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>150</v>
       </c>
     </row>
@@ -2272,19 +2331,19 @@
       <c r="C27">
         <v>4480</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <v>335</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="11">
         <v>50</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>243</v>
       </c>
       <c r="G27">
         <v>3450</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>159</v>
       </c>
     </row>
@@ -2298,19 +2357,19 @@
       <c r="C28">
         <v>5620</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>556</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="11">
         <v>118</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>406</v>
       </c>
       <c r="G28">
         <v>3840</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>205</v>
       </c>
     </row>
@@ -2324,19 +2383,19 @@
       <c r="C29">
         <v>6580</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <v>802</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="11">
         <v>200</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>503</v>
       </c>
       <c r="G29">
         <v>4090</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>284</v>
       </c>
     </row>
@@ -2350,19 +2409,19 @@
       <c r="C30">
         <v>7780</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="3">
         <v>1230</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="11">
         <v>333</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>738</v>
       </c>
       <c r="G30">
         <v>4120</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>359</v>
       </c>
     </row>
@@ -2376,19 +2435,19 @@
       <c r="C31">
         <v>8930</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <v>1720</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="11">
         <v>547</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>1030</v>
       </c>
       <c r="G31">
         <v>4310</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>443</v>
       </c>
     </row>
@@ -2402,19 +2461,19 @@
       <c r="C32">
         <v>10700</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="3">
         <v>2190</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="11">
         <v>815</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>1490</v>
       </c>
       <c r="G32">
         <v>4760</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>548</v>
       </c>
     </row>
@@ -2428,19 +2487,19 @@
       <c r="C33">
         <v>13300</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <v>3240</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="11">
         <v>1460</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>2460</v>
       </c>
       <c r="G33">
         <v>5040</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>606</v>
       </c>
     </row>
@@ -2454,19 +2513,19 @@
       <c r="C34">
         <v>16000</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>4270</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="11">
         <v>2120</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>3880</v>
       </c>
       <c r="G34">
         <v>5110</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>735</v>
       </c>
     </row>

</xml_diff>